<commit_message>
Add the excel file
</commit_message>
<xml_diff>
--- a/EXCEL.xlsx
+++ b/EXCEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75bb3638459a292f/Desktop/GIT PRACTICE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC104820E99C797C5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7CD0129-5821-4CB5-81B3-AB0A5771233D}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC104820E99C797C5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9893BCE2-7880-48A9-B799-EE3A2DC67D4B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,6 +72,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,10 +341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -370,46 +374,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Execel file is been updated
</commit_message>
<xml_diff>
--- a/EXCEL.xlsx
+++ b/EXCEL.xlsx
@@ -8,20 +8,58 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75bb3638459a292f/Desktop/GIT PRACTICE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC104820E99C797C5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9893BCE2-7880-48A9-B799-EE3A2DC67D4B}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="11_F25DC773A252ABDACC104820E99C797C5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66CA439D-8D9A-4BDA-A2E7-EED9DF58E63B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>NO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME </t>
+  </si>
+  <si>
+    <t>Harsh</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Swayam</t>
+  </si>
+  <si>
+    <t>Yugveer</t>
+  </si>
+  <si>
+    <t>Akshit</t>
+  </si>
+  <si>
+    <t>Persentage</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +93,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72,6 +116,1071 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38075117370892025"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1813163206084388"/>
+          <c:y val="0.11076206831454653"/>
+          <c:w val="0.82220438464609402"/>
+          <c:h val="0.71797551317645991"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Persentage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$2:$B$6</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Harsh</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Raj</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Swayam</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Yugveer</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Akshit</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E454-4869-B4FE-BAA3C64C1CE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1759998511"/>
+        <c:axId val="1760003311"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1759998511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1760003311"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1760003311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1759998511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCB4A654-8EC4-01BA-D1D9-4998B379D282}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,40 +1450,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1">
+        <v>92</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="1">
+        <v>75</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="1">
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>